<commit_message>
working version of tesseract
</commit_message>
<xml_diff>
--- a/test/1_output.xlsx
+++ b/test/1_output.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -35,20 +35,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FF0000"/>
         <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -64,11 +58,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,16 +438,15 @@
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="6" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="5" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Theo</t>
+          <t>Théo</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
@@ -462,9 +454,9 @@
           <t>Pre</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>%Theo</t>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>“Théo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -472,70 +464,80 @@
           <t>Post</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>%Theo</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>D%Post/Pre</t>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>“Théo</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>D%PostiPré</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Date test</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
           <t>21.02.22</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>21.02.22</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Heure test</t>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Heure</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>11:51</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>12:12</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Substance</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>‘Substance</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Ventoline</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>CVF</t>
         </is>
       </c>
-      <c r="B5" s="1" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>3.85</t>
         </is>
@@ -545,7 +547,7 @@
           <t>2.84</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>74</t>
         </is>
@@ -560,19 +562,14 @@
           <t>83</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>VEMS</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>veEMS</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>2.99</t>
         </is>
@@ -582,39 +579,34 @@
           <t>2.49</t>
         </is>
       </c>
-      <c r="D6" s="1" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>83</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>2.67</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>89</t>
         </is>
       </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>VEMS%CV</t>
         </is>
       </c>
-      <c r="B7" s="1" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>75.33</t>
         </is>
       </c>
-      <c r="C7" s="1" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>87.65</t>
         </is>
@@ -624,19 +616,14 @@
           <t>116</t>
         </is>
       </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>83.50</t>
-        </is>
-      </c>
-      <c r="F7" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>-5</t>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>83,50</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>"1</t>
         </is>
       </c>
     </row>
@@ -646,17 +633,17 @@
           <t>DEP</t>
         </is>
       </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>7.87</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>787</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>9.41</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D8" s="1" t="inlineStr">
         <is>
           <t>120</t>
         </is>
@@ -666,63 +653,53 @@
           <t>9.37</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>119</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>-0</t>
-        </is>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>DEM75</t>
         </is>
       </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>1.43</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>1.28</t>
         </is>
       </c>
-      <c r="D9" s="1" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>89</t>
         </is>
       </c>
-      <c r="E9" s="1" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>1.12</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>78</t>
         </is>
       </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>-12</t>
-        </is>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>DEM50</t>
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>DEMs0</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>4.12</t>
+          <t>4.42</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
@@ -730,9 +707,9 @@
           <t>3.93</t>
         </is>
       </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>96</t>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>95</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
@@ -745,51 +722,41 @@
           <t>82</t>
         </is>
       </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>-14</t>
-        </is>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>DEM25</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>7.01</t>
         </is>
       </c>
-      <c r="C11" s="1" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>7.82</t>
         </is>
       </c>
-      <c r="D11" s="1" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>112</t>
         </is>
       </c>
-      <c r="E11" s="1" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>7.67</t>
         </is>
       </c>
-      <c r="F11" s="1" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>109</t>
         </is>
       </c>
-      <c r="G11" s="1" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>DEMM</t>
         </is>
@@ -799,36 +766,31 @@
           <t>3.20</t>
         </is>
       </c>
-      <c r="C12" s="1" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>3.22</t>
         </is>
       </c>
-      <c r="D12" s="1" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>101</t>
         </is>
       </c>
-      <c r="E12" s="1" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>2.92</t>
         </is>
       </c>
-      <c r="F12" s="1" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="inlineStr">
-        <is>
-          <t>-10</t>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>DIM50</t>
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>DIMs0</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
@@ -836,100 +798,80 @@
           <t>3.10</t>
         </is>
       </c>
-      <c r="C13" s="1" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>3.27</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>VIMS</t>
-        </is>
-      </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>vims</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>2.34</t>
         </is>
       </c>
-      <c r="C14" s="1" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>2.37</t>
         </is>
       </c>
-      <c r="D14" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>DIP</t>
         </is>
       </c>
-      <c r="B15" s="1" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>3.30</t>
         </is>
       </c>
-      <c r="C15" s="1" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>3.33</t>
         </is>
       </c>
-      <c r="D15" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>VIMS%F</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>viMs%</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>96.66</t>
         </is>
       </c>
-      <c r="C16" s="1" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>96.34</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t>-0</t>
-        </is>
-      </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>CV max</t>
-        </is>
-      </c>
-      <c r="B17" s="1" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Vmax</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>3.99</t>
         </is>
       </c>
-      <c r="C17" s="1" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>3.25</t>
         </is>
       </c>
-      <c r="D17" s="1" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
         <is>
           <t>81</t>
         </is>
@@ -941,46 +883,46 @@
           <t>VRE</t>
         </is>
       </c>
-      <c r="B18" s="1" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>1.05</t>
         </is>
       </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>0.71</t>
-        </is>
-      </c>
-      <c r="D18" s="1" t="inlineStr">
-        <is>
-          <t>89</t>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>071</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>68</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>CRF-He</t>
         </is>
       </c>
-      <c r="B19" s="1" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>3.53</t>
         </is>
       </c>
-      <c r="C19" s="1" t="inlineStr">
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>2.22</t>
         </is>
       </c>
-      <c r="D19" s="1" t="inlineStr">
+      <c r="D19" s="2" t="inlineStr">
         <is>
           <t>63</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>VR</t>
         </is>
@@ -990,12 +932,12 @@
           <t>2.48</t>
         </is>
       </c>
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>1.51</t>
-        </is>
-      </c>
-      <c r="D20" s="1" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>1.81</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
         <is>
           <t>61</t>
         </is>
@@ -1004,51 +946,51 @@
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>CI</t>
-        </is>
-      </c>
-      <c r="B21" s="1" t="inlineStr">
+          <t>cl</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>2.94</t>
         </is>
       </c>
-      <c r="C21" s="3" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>2.54</t>
         </is>
       </c>
-      <c r="D21" s="1" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>86</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>CPT</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>cPT</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>6.66</t>
         </is>
       </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t>4.76</t>
-        </is>
-      </c>
-      <c r="D22" s="1" t="inlineStr">
-        <is>
-          <t>71</t>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>476</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>ial</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>VR%CPT</t>
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>VRYCPT</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
@@ -1056,68 +998,68 @@
           <t>39.70</t>
         </is>
       </c>
-      <c r="C23" s="1" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>31.74</t>
         </is>
       </c>
-      <c r="D23" s="1" t="inlineStr">
-        <is>
-          <t>08</t>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>80</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>DLCO_SB</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>8.72</t>
-        </is>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>DLCO_sB</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>872</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>6.45</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr">
         <is>
           <t>74</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>KCO_SB</t>
-        </is>
-      </c>
-      <c r="B25" s="1" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>KcO_sB</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>1.31</t>
         </is>
       </c>
-      <c r="C25" s="3" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>1.44</t>
         </is>
       </c>
-      <c r="D25" s="1" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr">
         <is>
           <t>110</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>VIN_SB</t>
         </is>
       </c>
-      <c r="B26" s="1" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>3.99</t>
         </is>
@@ -1134,46 +1076,36 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>VA_SB</t>
         </is>
       </c>
-      <c r="B27" s="1" t="inlineStr">
-        <is>
-          <t>6.51</t>
-        </is>
-      </c>
-      <c r="C27" s="1" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>651</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>4.48</t>
         </is>
       </c>
-      <c r="D27" s="1" t="inlineStr">
+      <c r="D27" s="2" t="inlineStr">
         <is>
           <t>69</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>CRF%CPT</t>
-        </is>
-      </c>
-      <c r="B28" s="1" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
-      </c>
-      <c r="C28" s="1" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>CRFYCPT</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>48</t>
-        </is>
-      </c>
-      <c r="D28" s="2" t="inlineStr">
-        <is>
-          <t>84</t>
         </is>
       </c>
     </row>
@@ -1183,21 +1115,21 @@
           <t>Hb</t>
         </is>
       </c>
-      <c r="B29" s="1" t="inlineStr">
+      <c r="B29" s="2" t="inlineStr">
         <is>
           <t>14.60</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>DLCOcSB</t>
-        </is>
-      </c>
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t>8.72</t>
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>DLCOcsB.</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>872</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
@@ -1205,29 +1137,29 @@
           <t>6.45</t>
         </is>
       </c>
-      <c r="D30" s="1" t="inlineStr">
+      <c r="D30" s="2" t="inlineStr">
         <is>
           <t>74</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>KCOc</t>
-        </is>
-      </c>
-      <c r="B31" s="1" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>KcOc</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>1.31</t>
         </is>
       </c>
-      <c r="C31" s="1" t="inlineStr">
+      <c r="C31" s="2" t="inlineStr">
         <is>
           <t>1.44</t>
         </is>
       </c>
-      <c r="D31" s="1" t="inlineStr">
+      <c r="D31" s="2" t="inlineStr">
         <is>
           <t>110</t>
         </is>

</xml_diff>

<commit_message>
fix: progress bars and implemented preloading of ocr models
</commit_message>
<xml_diff>
--- a/test/1_output.xlsx
+++ b/test/1_output.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,10 +444,11 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="9" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="6" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="5" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,14 +457,14 @@
           <t>Theo</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Pre</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>%oTheo</t>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>%Theo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -471,36 +472,31 @@
           <t>Post</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>"{oTheo</t>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%Theo</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>D"PostPre</t>
+          <t>D%Post/Pre</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Date</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Date test</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>est</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>02.22</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>21,02.22</t>
+          <t>21.02.22</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>21.02.22</t>
         </is>
       </c>
     </row>
@@ -510,14 +506,14 @@
           <t>Heure test</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>11.51</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>12.12</t>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>12:12</t>
         </is>
       </c>
     </row>
@@ -527,7 +523,7 @@
           <t>Substance</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Ventoline</t>
         </is>
@@ -544,9 +540,29 @@
           <t>3.85</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>2.84</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>13</t>
         </is>
       </c>
     </row>
@@ -558,7 +574,7 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>299</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -566,31 +582,61 @@
           <t>2.49</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
         <is>
           <t>2.67</t>
         </is>
       </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>VEMSPCV</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>75,33</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>VEMS%CV</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>75.33</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>87.65</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
+          <t>116</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
           <t>83.50</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>-5</t>
         </is>
       </c>
     </row>
@@ -602,26 +648,106 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
+          <t>7.87</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>9.41</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
           <t>120</t>
         </is>
       </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>9.37</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>DEM75</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>612</t>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>1.12</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t>-12</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>DEMSO</t>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>DEM50</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>4.12</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>3.93</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>3.37</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>-14</t>
         </is>
       </c>
     </row>
@@ -631,14 +757,34 @@
           <t>DEM25</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>7.01</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
+          <t>7.82</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr">
+        <is>
+          <t>7.67</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
           <t>109</t>
+        </is>
+      </c>
+      <c r="G11" s="1" t="inlineStr">
+        <is>
+          <t>-2</t>
         </is>
       </c>
     </row>
@@ -650,14 +796,54 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
           <t>101</t>
         </is>
       </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>2.92</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>-10</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>DIMSO</t>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>DIM50</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>3.10</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>3.27</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -667,6 +853,21 @@
           <t>VIMS</t>
         </is>
       </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>2.34</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -674,6 +875,21 @@
           <t>DIP</t>
         </is>
       </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>3.30</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>3.33</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -686,11 +902,36 @@
           <t>96.66</t>
         </is>
       </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>96.34</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>CV max</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>3.99</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>81</t>
         </is>
       </c>
     </row>
@@ -700,6 +941,21 @@
           <t>VRE</t>
         </is>
       </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>1.05</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>0.71</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -707,101 +963,273 @@
           <t>CRF-He</t>
         </is>
       </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>3.53</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>2.22</t>
+        </is>
+      </c>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
+          <t>VR</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
           <t>2.48</t>
         </is>
       </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>1.51</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>CI</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>2.94</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>2.54</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>CPT</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>6.66</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
         <is>
           <t>4.76</t>
         </is>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>VR"CPT</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>39.70</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>31.74</t>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>71</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>DLCO_</t>
+          <t>VR%CPT</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>39.70</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>31.74</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>08</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>KcO</t>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>DLCO_SB</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>8.72</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>6.45</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>74</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>VIN</t>
+          <t>KCO_SB</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>1.31</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>110</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>VIN_SB</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>3.99</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>3.19</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>VA_SB</t>
         </is>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>CRFOCPT</t>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>6.51</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>4.48</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>69</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="inlineStr">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>CRF%CPT</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Hb</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
         <is>
           <t>14.60</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="3" t="inlineStr">
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
         <is>
           <t>DLCOcSB</t>
         </is>
       </c>
-      <c r="B29" s="3" t="inlineStr">
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>8.72</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
         <is>
           <t>6.45</t>
         </is>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
+      <c r="D30" s="1" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
         <is>
           <t>KCOc</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>1.31</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>110</t>
         </is>
       </c>
     </row>

</xml_diff>